<commit_message>
common backup for unknown undate
</commit_message>
<xml_diff>
--- a/Fortran code/Fortran_bcs_pin_ettore/Record/1.2_compare/compare 1.2 48.xlsx
+++ b/Fortran code/Fortran_bcs_pin_ettore/Record/1.2_compare/compare 1.2 48.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{98775DBA-F2BC-4262-9806-391EA4DCBD55}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C0436994-76DF-4756-9FC1-3918F869D2F3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2567,115 +2567,6 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>DET</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]Sheet1!$X$230:$AR$230</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>-32.993838682204434</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-32.996675510826222</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-33.001192259065284</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-33.001829817882495</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-33.007158495644362</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-33.005856661110201</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-33.006848111317126</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-33.010016286983031</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-33.007666951946376</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-33.018805288272894</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-33.005632524770398</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-33.012919907986749</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-33.018867076897479</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-33.026816691405728</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-33.025721612904718</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-33.028213205832976</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-33.029017429124863</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-33.020953670632579</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-33.031453608230848</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-33.036028760991698</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-33.040787614380875</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4A88-4925-B680-BAB2BBE6BC7B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
@@ -2785,15 +2676,14 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:v>Analytic</c:v>
-          </c:tx>
+          <c:idx val="7"/>
+          <c:order val="7"/>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2804,11 +2694,15 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent6"/>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2816,72 +2710,72 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$117:$V$117</c:f>
+              <c:f>Sheet1!$B$46:$V$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-32.989975207364616</c:v>
+                  <c:v>-32.993838682204434</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-33.017900810561933</c:v>
+                  <c:v>-32.996675510826222</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-33.035083063623119</c:v>
+                  <c:v>-33.001192259065284</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-33.052163504800596</c:v>
+                  <c:v>-33.001829817882495</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-33.085450659107629</c:v>
+                  <c:v>-33.007158495644362</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-33.086037304383815</c:v>
+                  <c:v>-33.005856661110201</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-33.085105815269429</c:v>
+                  <c:v>-33.006848111317126</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-33.081528512005129</c:v>
+                  <c:v>-33.010016286983031</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-33.072460376226203</c:v>
+                  <c:v>-33.007666951946376</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-33.09973545780128</c:v>
+                  <c:v>-33.018805288272894</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-33.082198625358011</c:v>
+                  <c:v>-33.005632524770398</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-33.08296104456192</c:v>
+                  <c:v>-33.012919907986749</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-33.07691873724302</c:v>
+                  <c:v>-33.018867076897479</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-33.061201970302889</c:v>
+                  <c:v>-33.026816691405728</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-33.073615014219449</c:v>
+                  <c:v>-33.025721612904718</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-33.094847485282152</c:v>
+                  <c:v>-33.028213205832976</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-33.089763469275013</c:v>
+                  <c:v>-33.029017429124863</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-33.062802173115408</c:v>
+                  <c:v>-33.020953670632579</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-33.063735120516398</c:v>
+                  <c:v>-33.031453608230848</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-33.071016716084678</c:v>
+                  <c:v>-33.036028760991698</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-33.084500744923488</c:v>
+                  <c:v>-33.040787614380875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2889,7 +2783,119 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-4A88-4925-B680-BAB2BBE6BC7B}"/>
+              <c16:uniqueId val="{00000000-051A-4233-8682-0E32E2BD9EC6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$118:$V$118</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-32.989975207364616</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-33.017900810561933</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-33.035083063623119</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-33.052163504800596</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-33.085450659107629</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-33.086037304383815</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-33.085105815269429</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-33.081528512005129</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-33.072460376226203</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-33.09973545780128</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-33.082198625358011</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-33.08296104456192</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-33.07691873724302</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-33.061201970302889</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-33.073615014219449</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-33.094847485282152</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-33.089763469275013</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-33.062802173115408</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-33.063735120516398</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-33.071016716084678</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-33.084500744923488</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-051A-4233-8682-0E32E2BD9EC6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3020,6 +3026,123 @@
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-4A88-4925-B680-BAB2BBE6BC7B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:v>DET</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet1!$X$230:$AR$230</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="21"/>
+                      <c:pt idx="0">
+                        <c:v>-32.993838682204434</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-32.996675510826222</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>-33.001192259065284</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-33.001829817882495</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-33.007158495644362</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-33.005856661110201</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-33.006848111317126</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-33.010016286983031</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>-33.007666951946376</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>-33.018805288272894</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>-33.005632524770398</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>-33.012919907986749</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>-33.018867076897479</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>-33.026816691405728</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>-33.025721612904718</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>-33.028213205832976</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>-33.029017429124863</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>-33.020953670632579</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>-33.031453608230848</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>-33.036028760991698</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>-33.040787614380875</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-4A88-4925-B680-BAB2BBE6BC7B}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -3174,7 +3297,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>[1]Sheet1!$X$279:$AR$279</c15:sqref>
@@ -3251,9 +3374,126 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-4A88-4925-B680-BAB2BBE6BC7B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="5"/>
+                <c:tx>
+                  <c:v>Analytic</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent6"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent6"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$B$118:$V$118</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="21"/>
+                      <c:pt idx="0">
+                        <c:v>-32.989975207364616</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-33.017900810561933</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>-33.035083063623119</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>-33.052163504800596</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>-33.085450659107629</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>-33.086037304383815</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>-33.085105815269429</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>-33.081528512005129</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>-33.072460376226203</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>-33.09973545780128</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>-33.082198625358011</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>-33.08296104456192</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>-33.07691873724302</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>-33.061201970302889</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>-33.073615014219449</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>-33.094847485282152</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>-33.089763469275013</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>-33.062802173115408</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>-33.063735120516398</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>-33.071016716084678</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>-33.084500744923488</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000004-4A88-4925-B680-BAB2BBE6BC7B}"/>
+                    <c16:uniqueId val="{00000005-4A88-4925-B680-BAB2BBE6BC7B}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -3297,7 +3537,7 @@
                 </c:marker>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$B$140:$V$140</c15:sqref>
@@ -3374,7 +3614,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-6B6C-4823-878E-6B17864886CF}"/>
                   </c:ext>
@@ -8512,12 +8752,12 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>64941</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>61480</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>355023</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>25977</xdr:rowOff>
     </xdr:to>
@@ -9962,10 +10202,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:FC140"/>
+  <dimension ref="A1:FC187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X26" sqref="X26"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -24503,89 +24743,89 @@
       </c>
     </row>
     <row r="45" spans="1:93" x14ac:dyDescent="0.2">
-      <c r="B45" s="1">
-        <f t="shared" ref="B45:V45" si="7">AVERAGE(B25:B44)</f>
-        <v>-32.993838682204434</v>
-      </c>
-      <c r="C45" s="1">
+      <c r="B45">
+        <f>STDEV(B25:B44)</f>
+        <v>2.0062377854308516E-2</v>
+      </c>
+      <c r="C45">
+        <f t="shared" ref="C45:V45" si="7">STDEV(C25:C44)</f>
+        <v>1.8405783667998513E-2</v>
+      </c>
+      <c r="D45">
         <f t="shared" si="7"/>
-        <v>-32.996675510826222</v>
-      </c>
-      <c r="D45" s="1">
+        <v>1.9335410701481495E-2</v>
+      </c>
+      <c r="E45">
         <f t="shared" si="7"/>
-        <v>-33.001192259065284</v>
-      </c>
-      <c r="E45" s="1">
+        <v>2.1411374668709349E-2</v>
+      </c>
+      <c r="F45">
         <f t="shared" si="7"/>
-        <v>-33.001829817882495</v>
-      </c>
-      <c r="F45" s="1">
+        <v>1.4776998648175015E-2</v>
+      </c>
+      <c r="G45">
         <f t="shared" si="7"/>
-        <v>-33.007158495644362</v>
-      </c>
-      <c r="G45" s="1">
+        <v>2.3074604887966355E-2</v>
+      </c>
+      <c r="H45">
         <f t="shared" si="7"/>
-        <v>-33.005856661110201</v>
-      </c>
-      <c r="H45" s="1">
+        <v>2.381756481913315E-2</v>
+      </c>
+      <c r="I45">
         <f t="shared" si="7"/>
-        <v>-33.006848111317126</v>
-      </c>
-      <c r="I45" s="1">
+        <v>2.3417178365974827E-2</v>
+      </c>
+      <c r="J45">
         <f t="shared" si="7"/>
-        <v>-33.010016286983031</v>
-      </c>
-      <c r="J45" s="1">
+        <v>1.4669666538378687E-2</v>
+      </c>
+      <c r="K45">
         <f t="shared" si="7"/>
-        <v>-33.007666951946376</v>
-      </c>
-      <c r="K45" s="1">
+        <v>1.4583994660004103E-2</v>
+      </c>
+      <c r="L45">
         <f t="shared" si="7"/>
-        <v>-33.018805288272894</v>
-      </c>
-      <c r="L45" s="1">
+        <v>1.6340978696800505E-2</v>
+      </c>
+      <c r="M45">
         <f t="shared" si="7"/>
-        <v>-33.005632524770398</v>
-      </c>
-      <c r="M45" s="1">
+        <v>1.53426848902445E-2</v>
+      </c>
+      <c r="N45">
         <f t="shared" si="7"/>
-        <v>-33.012919907986749</v>
-      </c>
-      <c r="N45" s="1">
+        <v>2.0729110671667002E-2</v>
+      </c>
+      <c r="O45">
         <f t="shared" si="7"/>
-        <v>-33.018867076897479</v>
-      </c>
-      <c r="O45" s="1">
+        <v>1.8668630414265776E-2</v>
+      </c>
+      <c r="P45">
         <f t="shared" si="7"/>
-        <v>-33.026816691405728</v>
-      </c>
-      <c r="P45" s="1">
+        <v>2.3048688105790315E-2</v>
+      </c>
+      <c r="Q45">
         <f t="shared" si="7"/>
-        <v>-33.025721612904718</v>
-      </c>
-      <c r="Q45" s="1">
+        <v>1.7636015915231909E-2</v>
+      </c>
+      <c r="R45">
         <f t="shared" si="7"/>
-        <v>-33.028213205832976</v>
-      </c>
-      <c r="R45" s="1">
+        <v>1.4067695251933646E-2</v>
+      </c>
+      <c r="S45">
         <f t="shared" si="7"/>
-        <v>-33.029017429124863</v>
-      </c>
-      <c r="S45" s="1">
+        <v>1.6654009036771285E-2</v>
+      </c>
+      <c r="T45">
         <f t="shared" si="7"/>
-        <v>-33.020953670632579</v>
-      </c>
-      <c r="T45" s="1">
+        <v>2.1265217849602992E-2</v>
+      </c>
+      <c r="U45">
         <f t="shared" si="7"/>
-        <v>-33.031453608230848</v>
-      </c>
-      <c r="U45" s="1">
+        <v>1.7239049545916308E-2</v>
+      </c>
+      <c r="V45">
         <f t="shared" si="7"/>
-        <v>-33.036028760991698</v>
-      </c>
-      <c r="V45" s="1">
-        <f t="shared" si="7"/>
-        <v>-33.040787614380875</v>
+        <v>1.9508599117124978E-2</v>
       </c>
       <c r="Z45">
         <v>-24.713261872092399</v>
@@ -24800,6 +25040,90 @@
       <c r="CO45" s="1"/>
     </row>
     <row r="46" spans="1:93" x14ac:dyDescent="0.2">
+      <c r="B46" s="1">
+        <f>AVERAGE(B25:B44)</f>
+        <v>-32.993838682204434</v>
+      </c>
+      <c r="C46" s="1">
+        <f>AVERAGE(C25:C44)</f>
+        <v>-32.996675510826222</v>
+      </c>
+      <c r="D46" s="1">
+        <f>AVERAGE(D25:D44)</f>
+        <v>-33.001192259065284</v>
+      </c>
+      <c r="E46" s="1">
+        <f>AVERAGE(E25:E44)</f>
+        <v>-33.001829817882495</v>
+      </c>
+      <c r="F46" s="1">
+        <f>AVERAGE(F25:F44)</f>
+        <v>-33.007158495644362</v>
+      </c>
+      <c r="G46" s="1">
+        <f>AVERAGE(G25:G44)</f>
+        <v>-33.005856661110201</v>
+      </c>
+      <c r="H46" s="1">
+        <f>AVERAGE(H25:H44)</f>
+        <v>-33.006848111317126</v>
+      </c>
+      <c r="I46" s="1">
+        <f>AVERAGE(I25:I44)</f>
+        <v>-33.010016286983031</v>
+      </c>
+      <c r="J46" s="1">
+        <f>AVERAGE(J25:J44)</f>
+        <v>-33.007666951946376</v>
+      </c>
+      <c r="K46" s="1">
+        <f>AVERAGE(K25:K44)</f>
+        <v>-33.018805288272894</v>
+      </c>
+      <c r="L46" s="1">
+        <f>AVERAGE(L25:L44)</f>
+        <v>-33.005632524770398</v>
+      </c>
+      <c r="M46" s="1">
+        <f>AVERAGE(M25:M44)</f>
+        <v>-33.012919907986749</v>
+      </c>
+      <c r="N46" s="1">
+        <f>AVERAGE(N25:N44)</f>
+        <v>-33.018867076897479</v>
+      </c>
+      <c r="O46" s="1">
+        <f>AVERAGE(O25:O44)</f>
+        <v>-33.026816691405728</v>
+      </c>
+      <c r="P46" s="1">
+        <f>AVERAGE(P25:P44)</f>
+        <v>-33.025721612904718</v>
+      </c>
+      <c r="Q46" s="1">
+        <f>AVERAGE(Q25:Q44)</f>
+        <v>-33.028213205832976</v>
+      </c>
+      <c r="R46" s="1">
+        <f>AVERAGE(R25:R44)</f>
+        <v>-33.029017429124863</v>
+      </c>
+      <c r="S46" s="1">
+        <f>AVERAGE(S25:S44)</f>
+        <v>-33.020953670632579</v>
+      </c>
+      <c r="T46" s="1">
+        <f>AVERAGE(T25:T44)</f>
+        <v>-33.031453608230848</v>
+      </c>
+      <c r="U46" s="1">
+        <f>AVERAGE(U25:U44)</f>
+        <v>-33.036028760991698</v>
+      </c>
+      <c r="V46" s="1">
+        <f>AVERAGE(V25:V44)</f>
+        <v>-33.040787614380875</v>
+      </c>
       <c r="Z46">
         <v>-24.795378412263201</v>
       </c>
@@ -37037,259 +37361,345 @@
       </c>
     </row>
     <row r="117" spans="1:70" x14ac:dyDescent="0.2">
-      <c r="B117" s="1">
-        <f t="shared" ref="B117:M117" si="17">AVERAGE(B97:B116)</f>
-        <v>-32.989975207364616</v>
-      </c>
-      <c r="C117" s="1">
+      <c r="B117">
+        <f>STDEV(B97:B116)</f>
+        <v>1.8932676185113205E-2</v>
+      </c>
+      <c r="C117">
+        <f t="shared" ref="C117:V117" si="17">STDEV(C97:C116)</f>
+        <v>5.3101458423038241E-2</v>
+      </c>
+      <c r="D117">
         <f t="shared" si="17"/>
-        <v>-33.017900810561933</v>
-      </c>
-      <c r="D117" s="1">
+        <v>3.9033570639920086E-2</v>
+      </c>
+      <c r="E117">
         <f t="shared" si="17"/>
-        <v>-33.035083063623119</v>
-      </c>
-      <c r="E117" s="1">
+        <v>4.4623630177212652E-2</v>
+      </c>
+      <c r="F117">
         <f t="shared" si="17"/>
-        <v>-33.052163504800596</v>
-      </c>
-      <c r="F117" s="1">
+        <v>4.3947899945561378E-2</v>
+      </c>
+      <c r="G117">
         <f t="shared" si="17"/>
-        <v>-33.085450659107629</v>
-      </c>
-      <c r="G117" s="1">
+        <v>2.6820520085193186E-2</v>
+      </c>
+      <c r="H117">
         <f t="shared" si="17"/>
-        <v>-33.086037304383815</v>
-      </c>
-      <c r="H117" s="1">
+        <v>5.6827623905185434E-2</v>
+      </c>
+      <c r="I117">
         <f t="shared" si="17"/>
-        <v>-33.085105815269429</v>
-      </c>
-      <c r="I117" s="1">
+        <v>3.0194491032769728E-2</v>
+      </c>
+      <c r="J117">
         <f t="shared" si="17"/>
-        <v>-33.081528512005129</v>
-      </c>
-      <c r="J117" s="1">
+        <v>4.1726085663445593E-2</v>
+      </c>
+      <c r="K117">
         <f t="shared" si="17"/>
-        <v>-33.072460376226203</v>
-      </c>
-      <c r="K117" s="1">
+        <v>5.3075776616447093E-2</v>
+      </c>
+      <c r="L117">
         <f t="shared" si="17"/>
-        <v>-33.09973545780128</v>
-      </c>
-      <c r="L117" s="1">
+        <v>5.2073275837889919E-2</v>
+      </c>
+      <c r="M117">
         <f t="shared" si="17"/>
-        <v>-33.082198625358011</v>
-      </c>
-      <c r="M117" s="1">
+        <v>7.4263246769636609E-2</v>
+      </c>
+      <c r="N117">
         <f t="shared" si="17"/>
-        <v>-33.08296104456192</v>
-      </c>
-      <c r="N117" s="1">
-        <f t="shared" ref="N117:P117" si="18">AVERAGE(N97:N116)</f>
-        <v>-33.07691873724302</v>
-      </c>
-      <c r="O117" s="1">
-        <f t="shared" si="18"/>
-        <v>-33.061201970302889</v>
-      </c>
-      <c r="P117" s="1">
-        <f t="shared" si="18"/>
-        <v>-33.073615014219449</v>
-      </c>
-      <c r="Q117" s="1">
-        <f t="shared" ref="Q117:T117" si="19">AVERAGE(Q97:Q116)</f>
-        <v>-33.094847485282152</v>
-      </c>
-      <c r="R117" s="1">
-        <f t="shared" si="19"/>
-        <v>-33.089763469275013</v>
-      </c>
-      <c r="S117" s="1">
-        <f t="shared" si="19"/>
-        <v>-33.062802173115408</v>
-      </c>
-      <c r="T117" s="1">
-        <f t="shared" si="19"/>
-        <v>-33.063735120516398</v>
-      </c>
-      <c r="U117" s="1">
-        <f t="shared" ref="U117:V117" si="20">AVERAGE(U97:U116)</f>
-        <v>-33.071016716084678</v>
-      </c>
-      <c r="V117" s="1">
-        <f t="shared" si="20"/>
-        <v>-33.084500744923488</v>
+        <v>3.9763846708980775E-2</v>
+      </c>
+      <c r="O117">
+        <f t="shared" si="17"/>
+        <v>4.1977849839124483E-2</v>
+      </c>
+      <c r="P117">
+        <f t="shared" si="17"/>
+        <v>2.5723786803923249E-2</v>
+      </c>
+      <c r="Q117">
+        <f t="shared" si="17"/>
+        <v>2.9355588522274198E-2</v>
+      </c>
+      <c r="R117">
+        <f t="shared" si="17"/>
+        <v>2.2202854794152117E-2</v>
+      </c>
+      <c r="S117">
+        <f t="shared" si="17"/>
+        <v>3.4275363996596551E-2</v>
+      </c>
+      <c r="T117">
+        <f t="shared" si="17"/>
+        <v>3.2421333998308648E-2</v>
+      </c>
+      <c r="U117">
+        <f t="shared" si="17"/>
+        <v>3.9273263474959838E-2</v>
+      </c>
+      <c r="V117">
+        <f t="shared" si="17"/>
+        <v>3.8086434315664587E-2</v>
       </c>
       <c r="W117" s="1"/>
       <c r="Z117" s="1">
-        <f t="shared" ref="Z117:AP117" si="21">AVERAGE(Z97:Z116)</f>
+        <f t="shared" ref="Z117:AP117" si="18">AVERAGE(Z97:Z116)</f>
         <v>-24.518565912654616</v>
       </c>
       <c r="AA117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.509301301581022</v>
       </c>
       <c r="AB117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.633665885686959</v>
       </c>
       <c r="AC117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.569784509064334</v>
       </c>
       <c r="AD117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.614429327313651</v>
       </c>
       <c r="AE117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.635936268223642</v>
       </c>
       <c r="AF117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.566563106528104</v>
       </c>
       <c r="AG117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.470793858332378</v>
       </c>
       <c r="AH117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.496415794660585</v>
       </c>
       <c r="AI117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.446401826753153</v>
       </c>
       <c r="AJ117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.549815835957531</v>
       </c>
       <c r="AK117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.51218268798581</v>
       </c>
       <c r="AL117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.524727732226971</v>
       </c>
       <c r="AM117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.542752500098551</v>
       </c>
       <c r="AN117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.548541249947483</v>
       </c>
       <c r="AO117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.657216664596028</v>
       </c>
       <c r="AP117" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="18"/>
         <v>-24.545698358434475</v>
       </c>
       <c r="AQ117" s="1">
-        <f t="shared" ref="AQ117:AT117" si="22">AVERAGE(AQ97:AQ116)</f>
+        <f t="shared" ref="AQ117:AT117" si="19">AVERAGE(AQ97:AQ116)</f>
         <v>-24.517744747416355</v>
       </c>
       <c r="AR117" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>-24.522115377396442</v>
       </c>
       <c r="AS117" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>-24.522926866644298</v>
       </c>
       <c r="AT117" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>-24.530030383920391</v>
       </c>
       <c r="AU117" s="1"/>
       <c r="AX117" s="1">
-        <f t="shared" ref="AX117:BR117" si="23">AVERAGE(AX97:AX116)</f>
+        <f t="shared" ref="AX117:BR117" si="20">AVERAGE(AX97:AX116)</f>
         <v>-20.373597389832046</v>
       </c>
       <c r="AY117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.639912807488479</v>
       </c>
       <c r="AZ117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.884807812212564</v>
       </c>
       <c r="BA117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.820484200083207</v>
       </c>
       <c r="BB117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.861329534015169</v>
       </c>
       <c r="BC117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.742335163869058</v>
       </c>
       <c r="BD117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.989686288087618</v>
       </c>
       <c r="BE117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.743381173214484</v>
       </c>
       <c r="BF117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.433822508822679</v>
       </c>
       <c r="BG117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.4570825562189</v>
       </c>
       <c r="BH117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.766587904087455</v>
       </c>
       <c r="BI117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.651597099349711</v>
       </c>
       <c r="BJ117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.50446004174076</v>
       </c>
       <c r="BK117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.767350203172164</v>
       </c>
       <c r="BL117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.935994888729738</v>
       </c>
       <c r="BM117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.455830297915803</v>
       </c>
       <c r="BN117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.702061714368874</v>
       </c>
       <c r="BO117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.643853909644605</v>
       </c>
       <c r="BP117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.652573032660712</v>
       </c>
       <c r="BQ117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.724353646526399</v>
       </c>
       <c r="BR117" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="20"/>
         <v>-20.715311324916119</v>
+      </c>
+    </row>
+    <row r="118" spans="1:70" x14ac:dyDescent="0.2">
+      <c r="B118" s="1">
+        <f>AVERAGE(B97:B116)</f>
+        <v>-32.989975207364616</v>
+      </c>
+      <c r="C118" s="1">
+        <f>AVERAGE(C97:C116)</f>
+        <v>-33.017900810561933</v>
+      </c>
+      <c r="D118" s="1">
+        <f>AVERAGE(D97:D116)</f>
+        <v>-33.035083063623119</v>
+      </c>
+      <c r="E118" s="1">
+        <f>AVERAGE(E97:E116)</f>
+        <v>-33.052163504800596</v>
+      </c>
+      <c r="F118" s="1">
+        <f>AVERAGE(F97:F116)</f>
+        <v>-33.085450659107629</v>
+      </c>
+      <c r="G118" s="1">
+        <f>AVERAGE(G97:G116)</f>
+        <v>-33.086037304383815</v>
+      </c>
+      <c r="H118" s="1">
+        <f>AVERAGE(H97:H116)</f>
+        <v>-33.085105815269429</v>
+      </c>
+      <c r="I118" s="1">
+        <f>AVERAGE(I97:I116)</f>
+        <v>-33.081528512005129</v>
+      </c>
+      <c r="J118" s="1">
+        <f>AVERAGE(J97:J116)</f>
+        <v>-33.072460376226203</v>
+      </c>
+      <c r="K118" s="1">
+        <f>AVERAGE(K97:K116)</f>
+        <v>-33.09973545780128</v>
+      </c>
+      <c r="L118" s="1">
+        <f>AVERAGE(L97:L116)</f>
+        <v>-33.082198625358011</v>
+      </c>
+      <c r="M118" s="1">
+        <f>AVERAGE(M97:M116)</f>
+        <v>-33.08296104456192</v>
+      </c>
+      <c r="N118" s="1">
+        <f>AVERAGE(N97:N116)</f>
+        <v>-33.07691873724302</v>
+      </c>
+      <c r="O118" s="1">
+        <f>AVERAGE(O97:O116)</f>
+        <v>-33.061201970302889</v>
+      </c>
+      <c r="P118" s="1">
+        <f>AVERAGE(P97:P116)</f>
+        <v>-33.073615014219449</v>
+      </c>
+      <c r="Q118" s="1">
+        <f>AVERAGE(Q97:Q116)</f>
+        <v>-33.094847485282152</v>
+      </c>
+      <c r="R118" s="1">
+        <f>AVERAGE(R97:R116)</f>
+        <v>-33.089763469275013</v>
+      </c>
+      <c r="S118" s="1">
+        <f>AVERAGE(S97:S116)</f>
+        <v>-33.062802173115408</v>
+      </c>
+      <c r="T118" s="1">
+        <f>AVERAGE(T97:T116)</f>
+        <v>-33.063735120516398</v>
+      </c>
+      <c r="U118" s="1">
+        <f>AVERAGE(U97:U116)</f>
+        <v>-33.071016716084678</v>
+      </c>
+      <c r="V118" s="1">
+        <f>AVERAGE(V97:V116)</f>
+        <v>-33.084500744923488</v>
       </c>
     </row>
     <row r="119" spans="1:70" x14ac:dyDescent="0.2">
@@ -40825,238 +41235,448 @@
     </row>
     <row r="140" spans="2:69" x14ac:dyDescent="0.2">
       <c r="B140" s="1">
-        <f t="shared" ref="B140:S140" si="24">AVERAGE(B120:B139)</f>
+        <f t="shared" ref="B140:S140" si="21">AVERAGE(B120:B139)</f>
         <v>-32.925870810287414</v>
       </c>
       <c r="C140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.053872788372985</v>
       </c>
       <c r="D140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.071107966362078</v>
       </c>
       <c r="E140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.094712113328221</v>
       </c>
       <c r="F140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.067031254448331</v>
       </c>
       <c r="G140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.09054668154107</v>
       </c>
       <c r="H140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.078064384288005</v>
       </c>
       <c r="I140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.077803345760437</v>
       </c>
       <c r="J140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.082351503197508</v>
       </c>
       <c r="K140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.072609525375526</v>
       </c>
       <c r="L140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.100452648504962</v>
       </c>
       <c r="M140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.073152380549054</v>
       </c>
       <c r="N140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.063791290840797</v>
       </c>
       <c r="O140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.077243866105334</v>
       </c>
       <c r="P140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.072696945048015</v>
       </c>
       <c r="Q140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.079913904147986</v>
       </c>
       <c r="R140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.075309738041746</v>
       </c>
       <c r="S140" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="21"/>
         <v>-33.08277044957422</v>
       </c>
       <c r="T140" s="1">
-        <f t="shared" ref="T140:V140" si="25">AVERAGE(T120:T139)</f>
+        <f t="shared" ref="T140:V140" si="22">AVERAGE(T120:T139)</f>
         <v>-33.097977945672845</v>
       </c>
       <c r="U140" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>-33.090678925498807</v>
       </c>
       <c r="V140" s="1">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>-33.088476394869133</v>
       </c>
       <c r="W140" s="1"/>
       <c r="Z140" s="1">
-        <f t="shared" ref="Z140:AP140" si="26">AVERAGE(Z120:Z139)</f>
+        <f t="shared" ref="Z140:AP140" si="23">AVERAGE(Z120:Z139)</f>
         <v>-24.71696698975186</v>
       </c>
       <c r="AA140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.567420230492864</v>
       </c>
       <c r="AB140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.660333465426991</v>
       </c>
       <c r="AC140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.565528023039793</v>
       </c>
       <c r="AD140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.44900283975495</v>
       </c>
       <c r="AE140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.493532545544763</v>
       </c>
       <c r="AF140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.566265853082971</v>
       </c>
       <c r="AG140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.544755818125545</v>
       </c>
       <c r="AH140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.558869332646005</v>
       </c>
       <c r="AI140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.555332711234797</v>
       </c>
       <c r="AJ140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.508481230488918</v>
       </c>
       <c r="AK140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.496923921369472</v>
       </c>
       <c r="AL140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.584857604254417</v>
       </c>
       <c r="AM140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.575701382537709</v>
       </c>
       <c r="AN140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.463393727494104</v>
       </c>
       <c r="AO140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.534977490515963</v>
       </c>
       <c r="AP140" s="1">
-        <f t="shared" si="26"/>
+        <f t="shared" si="23"/>
         <v>-24.57906627998134</v>
       </c>
       <c r="AQ140" s="1"/>
       <c r="AX140" s="1">
-        <f t="shared" ref="AX140:BQ140" si="27">AVERAGE(AX120:AX139)</f>
+        <f t="shared" ref="AX140:BQ140" si="24">AVERAGE(AX120:AX139)</f>
         <v>-20.110420729901428</v>
       </c>
       <c r="AY140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.306528231734209</v>
       </c>
       <c r="AZ140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.37245996515356</v>
       </c>
       <c r="BA140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.386123149192276</v>
       </c>
       <c r="BB140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.451073095580792</v>
       </c>
       <c r="BC140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.342810641300524</v>
       </c>
       <c r="BD140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.092774058322306</v>
       </c>
       <c r="BE140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.538164782536622</v>
       </c>
       <c r="BF140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.430392934757553</v>
       </c>
       <c r="BG140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.2780972906965</v>
       </c>
       <c r="BH140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.291113511396652</v>
       </c>
       <c r="BI140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.009929569531867</v>
       </c>
       <c r="BJ140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.513993191342639</v>
       </c>
       <c r="BK140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.634337731630488</v>
       </c>
       <c r="BL140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.226499171080579</v>
       </c>
       <c r="BM140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.471022034770929</v>
       </c>
       <c r="BN140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.643668790547196</v>
       </c>
       <c r="BO140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.360698201434626</v>
       </c>
       <c r="BP140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.410533417496957</v>
       </c>
       <c r="BQ140" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="24"/>
         <v>-20.501226031609271</v>
+      </c>
+    </row>
+    <row r="167" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P167" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q167" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="168" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P168" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q168" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="169" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P169" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q169" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="170" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P170" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q170" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="171" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P171" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q171" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="172" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P172" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q172" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="173" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P173" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q173" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="174" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P174" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q174" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="175" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P175" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q175" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="176" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P176" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q176" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="177" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P177" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q177" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="178" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P178" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q178" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="179" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P179" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q179" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="180" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P180" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q180" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="181" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P181" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q181" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="182" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P182" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q182" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="183" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P183" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q183" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="184" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P184" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q184" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="185" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P185" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q185" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="186" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P186" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q186" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="187" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="P187" t="e">
+        <f>STDEV(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="Q187" s="1" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>